<commit_message>
fix some silkscreen errors, new gerber
</commit_message>
<xml_diff>
--- a/BOM/Inductor_BOM.xlsx
+++ b/BOM/Inductor_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Documents\KiCad\Projets\Dual_BPF\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAACC42E-25A9-494D-9A59-A17CFC08508C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EF26FD-59D2-48B5-81BF-9EC3FF9FDE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2430" yWindow="2235" windowWidth="18000" windowHeight="10740" xr2:uid="{FED2990D-BD65-4E03-A09B-9EF770CE9EA3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>inductance</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>TO-270-WB-4</t>
+  </si>
+  <si>
+    <t>en stock</t>
+  </si>
+  <si>
+    <t>pas nécessaire</t>
   </si>
 </sst>
 </file>
@@ -577,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E80346-6175-4F59-AA41-58E4BCAA1322}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +885,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -901,8 +907,11 @@
       <c r="G17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -922,10 +931,13 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F19">
         <f>SUM(F2:F18)</f>
         <v>279.56999999999994</v>
+      </c>
+      <c r="H19" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>